<commit_message>
Some more effort with the game work
</commit_message>
<xml_diff>
--- a/2_Homeworks/Game.xlsx
+++ b/2_Homeworks/Game.xlsx
@@ -494,7 +494,7 @@
   <dimension ref="E3:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -505,23 +505,23 @@
   <sheetData>
     <row r="3" spans="5:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="G3" s="5">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="5">
+        <v>-6</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5">
         <v>10</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5">
-        <v>30</v>
       </c>
       <c r="L3" s="3">
         <f>G3-I3+K3</f>
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="5:12" ht="23.25" x14ac:dyDescent="0.35">
@@ -544,23 +544,23 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="5">
-        <v>-4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="5">
-        <v>-25</v>
+        <v>7</v>
       </c>
       <c r="L5" s="3">
         <f>G5+I5+K5</f>
-        <v>-4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="5:12" ht="23.25" x14ac:dyDescent="0.35">
@@ -583,43 +583,43 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="5">
-        <v>-17</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K7" s="5">
-        <v>-18</v>
+        <v>1</v>
       </c>
       <c r="L7" s="3">
         <f>G7+I7-K7</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="5:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G8" s="3">
         <f>G3*G5+G7</f>
-        <v>-89</v>
+        <v>23</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3">
         <f>I3+I5*I7</f>
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3">
         <f>K3+K5-K7</f>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="L8" s="3">
         <f>G3+I5+K7</f>
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="5:12" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Some more effort with the algo
</commit_message>
<xml_diff>
--- a/2_Homeworks/Game.xlsx
+++ b/2_Homeworks/Game.xlsx
@@ -494,7 +494,7 @@
   <dimension ref="E3:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -511,17 +511,17 @@
         <v>0</v>
       </c>
       <c r="I3" s="5">
-        <v>-6</v>
+        <v>2</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L3" s="3">
         <f>G3-I3+K3</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="5:12" ht="23.25" x14ac:dyDescent="0.35">
@@ -544,13 +544,13 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>1</v>
@@ -583,19 +583,19 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="3">
         <f>G7+I7-K7</f>
@@ -605,7 +605,7 @@
     <row r="8" spans="5:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G8" s="3">
         <f>G3*G5+G7</f>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3">
@@ -615,7 +615,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3">
         <f>K3+K5-K7</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8" s="3">
         <f>G3+I5+K7</f>

</xml_diff>

<commit_message>
Wow finally solved the puzzle - Brute force is stupid as permutations will take way long time. Should've some other constraint based algo
</commit_message>
<xml_diff>
--- a/2_Homeworks/Game.xlsx
+++ b/2_Homeworks/Game.xlsx
@@ -46,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -87,8 +87,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +105,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -129,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -144,12 +157,554 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF008000"/>
+      <color rgb="FF00CC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -494,7 +1049,7 @@
   <dimension ref="E3:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -505,7 +1060,7 @@
   <sheetData>
     <row r="3" spans="5:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="G3" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>0</v>
@@ -517,9 +1072,9 @@
         <v>1</v>
       </c>
       <c r="K3" s="5">
-        <v>8</v>
-      </c>
-      <c r="L3" s="3">
+        <v>7</v>
+      </c>
+      <c r="L3" s="8">
         <f>G3-I3+K3</f>
         <v>10</v>
       </c>
@@ -538,7 +1093,7 @@
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="5:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E5" s="1"/>
@@ -550,15 +1105,15 @@
         <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="5">
-        <v>7</v>
-      </c>
-      <c r="L5" s="3">
+        <v>9</v>
+      </c>
+      <c r="L5" s="8">
         <f>G5+I5+K5</f>
         <v>19</v>
       </c>
@@ -577,47 +1132,47 @@
       <c r="K6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="5:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8">
         <f>G7+I7-K7</f>
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="5:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G8" s="3">
+      <c r="G8" s="8">
         <f>G3*G5+G7</f>
-        <v>20</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3">
+        <v>23</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="8">
         <f>I3+I5*I7</f>
         <v>50</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3">
+      <c r="J8" s="6"/>
+      <c r="K8" s="8">
         <f>K3+K5-K7</f>
         <v>15</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="8">
         <f>G3+I5+K7</f>
         <v>12</v>
       </c>
@@ -631,6 +1186,41 @@
       <c r="F10" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="L3">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="notEqual">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="notEqual">
+      <formula>19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="notEqual">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="notEqual">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="notEqual">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="notEqual">
+      <formula>50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="notEqual">
+      <formula>23</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>